<commit_message>
Third commmit for Readme
</commit_message>
<xml_diff>
--- a/output/option_valuation_results.xlsx
+++ b/output/option_valuation_results.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3/31/2022</t>
+          <t>1/10/2024</t>
         </is>
       </c>
     </row>
@@ -463,7 +463,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3/31/2022</t>
+          <t>7/10/2024</t>
         </is>
       </c>
     </row>
@@ -475,7 +475,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/31/2032</t>
+          <t>7/10/2025</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3/31/2026</t>
+          <t>1/10/2025</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>86.29000000000001</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>86.29000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0238</v>
+        <v>0.0522</v>
       </c>
     </row>
     <row r="10">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4976</v>
+        <v>0.2323</v>
       </c>
     </row>
     <row r="11">
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>45.9</v>
+        <v>55.34</v>
       </c>
     </row>
   </sheetData>
@@ -562,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,238 +578,48 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015-03-31 to 2022-03-31</t>
+          <t>2023-07-10 to 2024-07-10</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BKKT</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>160.88</v>
+        <v>22.05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FRGE</t>
+          <t>GOOG</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>80.04000000000001</v>
+        <v>27.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VIRT</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36.3</v>
+        <v>20.17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HOOD</t>
+          <t>Average</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>102.8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>COIN</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>63.99</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>33.78</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>MKTX</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>31.29</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>AMG</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>36.48</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>APO</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>36.85</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ARES</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>35.06</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>BX</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>33.73</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>OWL</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>44.53</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>BPT.L</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>47.24</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>CG</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>35.66</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>EQT.ST</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>52.15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>HLNE</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>36.84</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>KKR</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>34.45</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>EMG.L</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>31.66</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>PGHN.SW</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>24.05</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>PHLL.L</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>STEP</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>42.85</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>TPG</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>51.49</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Average</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>49.76</v>
+        <v>23.23</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +644,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2022-03-31</t>
+          <t>2024-07-10</t>
         </is>
       </c>
     </row>
@@ -845,7 +655,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.49</v>
+        <v>5.22</v>
       </c>
     </row>
     <row r="3">
@@ -855,7 +665,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.97</v>
+        <v>4.97</v>
       </c>
     </row>
     <row r="4">
@@ -865,7 +675,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.46</v>
+        <v>4.73</v>
       </c>
     </row>
     <row r="5">
@@ -875,7 +685,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.94</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="6">
@@ -885,7 +695,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.42</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="7">
@@ -895,7 +705,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.4</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +715,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.38</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="9">
@@ -915,7 +725,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.37</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="10">
@@ -925,7 +735,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.35</v>
+        <v>4.27</v>
       </c>
     </row>
     <row r="11">
@@ -935,7 +745,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.33</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="12">
@@ -945,7 +755,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.34</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="13">
@@ -955,7 +765,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.34</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="14">
@@ -965,7 +775,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.35</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="15">
@@ -975,7 +785,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.35</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="16">
@@ -985,7 +795,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.36</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="17">
@@ -995,7 +805,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2.37</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="18">
@@ -1005,7 +815,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2.37</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="19">
@@ -1015,7 +825,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.38</v>
+        <v>4.36</v>
       </c>
     </row>
     <row r="20">
@@ -1025,7 +835,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2.38</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="21">
@@ -1035,7 +845,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.39</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="22">
@@ -1045,7 +855,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2.4</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="23">
@@ -1055,7 +865,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2.4</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="24">
@@ -1065,7 +875,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2.41</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="25">
@@ -1075,7 +885,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2.41</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="26">
@@ -1085,7 +895,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.42</v>
+        <v>4.42</v>
       </c>
     </row>
     <row r="27">
@@ -1095,7 +905,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2.43</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="28">
@@ -1105,7 +915,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2.43</v>
+        <v>4.44</v>
       </c>
     </row>
     <row r="29">
@@ -1115,7 +925,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2.44</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="30">
@@ -1125,7 +935,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2.44</v>
+        <v>4.46</v>
       </c>
     </row>
     <row r="31">
@@ -1135,7 +945,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2.45</v>
+        <v>4.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made frequency parameter optional and updated README
</commit_message>
<xml_diff>
--- a/output/option_valuation_results.xlsx
+++ b/output/option_valuation_results.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1/10/2024</t>
+          <t>3/31/2022</t>
         </is>
       </c>
     </row>
@@ -463,7 +463,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7/10/2024</t>
+          <t>3/31/2022</t>
         </is>
       </c>
     </row>
@@ -475,7 +475,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>3/31/2032</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1/10/2025</t>
+          <t>3/31/2026</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>150</v>
+        <v>86.29000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>86.29000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0522</v>
+        <v>0.0238</v>
       </c>
     </row>
     <row r="10">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2323</v>
+        <v>0.4888</v>
       </c>
     </row>
     <row r="11">
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>55.34</v>
+        <v>45.31</v>
       </c>
     </row>
   </sheetData>
@@ -562,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,48 +578,238 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2023-07-10 to 2024-07-10</t>
+          <t>2015-03-31 to 2022-03-31</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>BKKT</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22.05</v>
+        <v>173.88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GOOG</t>
+          <t>FRGE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>27.48</v>
+        <v>87.97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>VIRT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20.17</v>
+        <v>37.77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>HOOD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>92.48999999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>54.53</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>31.39</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MKTX</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>31.08</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AMG</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>36.12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>APO</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>36.22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ARES</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>35.72</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BX</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>33.71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>OWL</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>39.56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BPT.L</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>46.92</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CG</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>34.74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>EQT.ST</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>52.54</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HLNE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>35.07</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>KKR</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>EMG.L</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>30.71</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PGHN.SW</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>25.04</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PHLL.L</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>50.09</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>STEP</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>45.23</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TPG</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>28.43</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>Average</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>23.23</v>
+      <c r="B24" t="n">
+        <v>48.88</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +834,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2022-03-31</t>
         </is>
       </c>
     </row>
@@ -655,7 +845,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.22</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="3">
@@ -665,7 +855,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.97</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="4">
@@ -675,7 +865,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.73</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="5">
@@ -685,7 +875,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.49</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="6">
@@ -695,7 +885,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.24</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="7">
@@ -705,7 +895,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.25</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="8">
@@ -715,7 +905,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.26</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +915,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4.26</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="10">
@@ -735,7 +925,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.27</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="11">
@@ -745,7 +935,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.28</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="12">
@@ -755,7 +945,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.29</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="13">
@@ -765,7 +955,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4.3</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="14">
@@ -775,7 +965,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.31</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="15">
@@ -785,7 +975,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.32</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="16">
@@ -795,7 +985,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4.33</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="17">
@@ -805,7 +995,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.34</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="18">
@@ -815,7 +1005,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.35</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="19">
@@ -825,7 +1015,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4.36</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="20">
@@ -835,7 +1025,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4.37</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="21">
@@ -845,7 +1035,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4.38</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="22">
@@ -855,7 +1045,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4.38</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="23">
@@ -865,7 +1055,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4.39</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="24">
@@ -875,7 +1065,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4.4</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="25">
@@ -885,7 +1075,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4.41</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="26">
@@ -895,7 +1085,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4.42</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="27">
@@ -905,7 +1095,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4.43</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="28">
@@ -915,7 +1105,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.44</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="29">
@@ -925,7 +1115,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4.45</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="30">
@@ -935,7 +1125,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4.46</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="31">
@@ -945,7 +1135,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4.47</v>
+        <v>2.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>